<commit_message>
Atualizou os títulos dos gráfico
</commit_message>
<xml_diff>
--- a/Gestao de estudo.xlsx
+++ b/Gestao de estudo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALDEVAN\Downloads\#Gestão Dos Estudos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALDEVAN\Downloads\#Gestão Dos Estudos\Controle-de-estudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A2AA47-0A9F-4BB0-9643-768696EFDAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8970" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking" sheetId="3" state="hidden" r:id="rId1"/>
@@ -27,9 +28,9 @@
     <definedName name="SegmentaçãodeDados_Semana">#N/A</definedName>
     <definedName name="SegmentaçãodeDados_Semana1">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId8"/>
+    <pivotCache cacheId="12" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -51,12 +52,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="125">
   <si>
     <t>Data</t>
   </si>
@@ -426,11 +436,17 @@
   <si>
     <t>Total Horas</t>
   </si>
+  <si>
+    <t>ago</t>
+  </si>
+  <si>
+    <t>Módulo 1: (NOVO) Primeiros Passos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="[$-416]dddd"/>
@@ -659,7 +675,459 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="91">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
     </dxf>
@@ -1924,7 +2392,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -1942,7 +2410,28 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total Mensal Por Curso</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2013,7 +2502,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2047,9 +2535,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -2143,7 +2629,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2202,6 +2687,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1E34-4CED-B383-E31055062121}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2213,11 +2703,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-828272224"/>
-        <c:axId val="-828266784"/>
+        <c:axId val="2125015824"/>
+        <c:axId val="2125002224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-828272224"/>
+        <c:axId val="2125015824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2257,7 +2747,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-828266784"/>
+        <c:crossAx val="2125002224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2265,7 +2755,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-828266784"/>
+        <c:axId val="2125002224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,7 +2789,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-828272224"/>
+        <c:crossAx val="2125015824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2313,7 +2803,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2385,7 +2874,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -2421,12 +2910,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Título</a:t>
+              <a:t>Evolução Por Dia</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2896,7 +3384,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="bg1">
@@ -2939,9 +3426,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -3056,7 +3541,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3242,6 +3726,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6651-4554-A653-8533AD70C864}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3253,11 +3742,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-828260256"/>
-        <c:axId val="-828266240"/>
+        <c:axId val="2125009840"/>
+        <c:axId val="2125010384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-828260256"/>
+        <c:axId val="2125009840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3297,7 +3786,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-828266240"/>
+        <c:crossAx val="2125010384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3305,7 +3794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-828266240"/>
+        <c:axId val="2125010384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3339,7 +3828,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-828260256"/>
+        <c:crossAx val="2125009840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3353,7 +3842,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3424,7 +3912,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -3460,12 +3948,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Título</a:t>
+              <a:t>Evolução Mensal</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3935,7 +4422,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="bg1">
@@ -3978,9 +4464,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -4095,7 +4579,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4115,9 +4598,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Evolucao mensal'!$A$4:$A$9</c:f>
+              <c:f>'Evolucao mensal'!$A$4:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>mar</c:v>
                 </c:pt>
@@ -4133,15 +4616,18 @@
                 <c:pt idx="4">
                   <c:v>jul</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>ago</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Evolucao mensal'!$B$4:$B$9</c:f>
+              <c:f>'Evolucao mensal'!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>[h]:mm:ss;@</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>2.2652777777777779</c:v>
                 </c:pt>
@@ -4157,10 +4643,18 @@
                 <c:pt idx="4">
                   <c:v>3.838194444444444</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6111111111111115E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C89B-4091-8A3C-C2E721F6C358}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4172,11 +4666,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-828263520"/>
-        <c:axId val="-828262976"/>
+        <c:axId val="2125010928"/>
+        <c:axId val="2125011472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-828263520"/>
+        <c:axId val="2125010928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4216,7 +4710,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-828262976"/>
+        <c:crossAx val="2125011472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4224,7 +4718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-828262976"/>
+        <c:axId val="2125011472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4258,7 +4752,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-828263520"/>
+        <c:crossAx val="2125010928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4272,7 +4766,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4343,7 +4836,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -4361,7 +4854,28 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total Geral Por Curso</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4503,7 +5017,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -4537,9 +5050,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
@@ -4633,7 +5144,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4729,7 +5239,7 @@
                   <c:v>4.6270833333333323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5562499999999999</c:v>
+                  <c:v>3.5923611111111109</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.40208333333333335</c:v>
@@ -4782,6 +5292,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-33C7-4134-8E37-C29C41428B66}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4793,11 +5308,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-828267872"/>
-        <c:axId val="-828257536"/>
+        <c:axId val="2125007120"/>
+        <c:axId val="2125007664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-828267872"/>
+        <c:axId val="2125007120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4837,7 +5352,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-828257536"/>
+        <c:crossAx val="2125007664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4845,7 +5360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-828257536"/>
+        <c:axId val="2125007664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4879,7 +5394,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-828267872"/>
+        <c:crossAx val="2125007120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4893,7 +5408,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7003,21 +7517,27 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>266</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>275</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Semana 1"/>
+            <xdr:cNvPr id="2" name="Semana 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -7031,7 +7551,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -7041,7 +7561,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11087100" y="2943225"/>
+              <a:off x="11029950" y="2724150"/>
               <a:ext cx="1409700" cy="1800225"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7062,8 +7582,8 @@
             <a:p>
               <a:r>
                 <a:rPr lang="pt-BR" sz="1100"/>
-                <a:t>Esta forma representa uma segmentação de dados de tabela. Segmentações de dados de tabela têm suporte no Excel 2013 ou em versões posteriores.
-Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho tiver sido salva no Excel 2007 ou em versões anteriores, a segmentação de dados não poderá ser usada.</a:t>
+                <a:t>Esta forma representa um slicer da tabela. As segmentações de dados da tabela não são suportadas nesta versão do Excel.
+Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho foi salva no Excel 2007 ou anterior, a segmentação de dados não pode ser usada.</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -7075,21 +7595,27 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>256</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>255</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>265</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="Referencia 1"/>
+            <xdr:cNvPr id="4" name="Referencia 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -7103,7 +7629,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -7113,7 +7639,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11077575" y="1028700"/>
+              <a:off x="11020425" y="809625"/>
               <a:ext cx="1390650" cy="1800225"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7134,8 +7660,8 @@
             <a:p>
               <a:r>
                 <a:rPr lang="pt-BR" sz="1100"/>
-                <a:t>Esta forma representa uma segmentação de dados de tabela. Segmentações de dados de tabela têm suporte no Excel 2013 ou em versões posteriores.
-Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho tiver sido salva no Excel 2007 ou em versões anteriores, a segmentação de dados não poderá ser usada.</a:t>
+                <a:t>Esta forma representa um slicer da tabela. As segmentações de dados da tabela não são suportadas nesta versão do Excel.
+Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho foi salva no Excel 2007 ou anterior, a segmentação de dados não pode ser usada.</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -7161,6 +7687,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Imagem 4">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -7210,7 +7741,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CaixaDeTexto 1"/>
+        <xdr:cNvPr id="2" name="CaixaDeTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7308,7 +7845,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 1"/>
+        <xdr:cNvPr id="3" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7326,19 +7869,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 1"/>
+        <xdr:cNvPr id="4" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7356,19 +7905,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Gráfico 1"/>
+        <xdr:cNvPr id="5" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7398,7 +7953,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="'Total geral por curso'!B1">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CaixaDeTexto 5"/>
+        <xdr:cNvPr id="6" name="CaixaDeTexto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7446,7 +8007,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>400:24:00</a:t>
+            <a:t>401:16:00</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -7475,7 +8036,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CaixaDeTexto 6"/>
+        <xdr:cNvPr id="7" name="CaixaDeTexto 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7559,7 +8126,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="Dados!A2">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CaixaDeTexto 7"/>
+        <xdr:cNvPr id="8" name="CaixaDeTexto 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7636,7 +8209,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CaixaDeTexto 8"/>
+        <xdr:cNvPr id="9" name="CaixaDeTexto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -7708,13 +8287,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:colOff>228601</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>514351</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
@@ -7722,7 +8301,13 @@
       <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="10" name="Referencia"/>
+            <xdr:cNvPr id="10" name="Referencia">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000A000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -7780,21 +8365,27 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
+      <xdr:colOff>342901</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>400052</xdr:colOff>
+      <xdr:colOff>161927</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="11" name="Semana"/>
+            <xdr:cNvPr id="11" name="Semana">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000B000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -7808,7 +8399,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -7818,7 +8409,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1800226" y="600075"/>
+              <a:off x="1276351" y="600075"/>
               <a:ext cx="4086226" cy="676275"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -7858,7 +8449,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>269025</xdr:colOff>
+      <xdr:colOff>297600</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>83926</xdr:rowOff>
     </xdr:to>
@@ -7866,7 +8457,13 @@
       <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="14" name="Data"/>
+            <xdr:cNvPr id="14" name="Data">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000E000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -7936,7 +8533,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="16" name="Gráfico 2"/>
+        <xdr:cNvPr id="16" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7968,6 +8571,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="17" name="Imagem 16">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000011000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -8001,13 +8609,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="ALDEVAN" refreshedDate="44772.548471643517" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="261">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="ALDEVAN" refreshedDate="44774.956184606483" createdVersion="5" refreshedVersion="7" minRefreshableVersion="3" recordCount="262" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="baseDeDados"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Data" numFmtId="167">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2022-03-09T00:00:00" maxDate="2022-07-31T00:00:00" count="113">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2022-03-09T00:00:00" maxDate="2022-08-02T00:00:00" count="114">
         <d v="2022-03-09T00:00:00"/>
         <d v="2022-03-10T00:00:00"/>
         <d v="2022-03-11T00:00:00"/>
@@ -8120,19 +8728,21 @@
         <d v="2022-07-27T00:00:00"/>
         <d v="2022-07-28T00:00:00"/>
         <d v="2022-07-29T00:00:00"/>
+        <d v="2022-08-01T00:00:00"/>
         <d v="2022-07-30T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Dia Semana" numFmtId="165">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2022-03-09T00:00:00" maxDate="2022-07-30T00:00:00"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2022-03-09T00:00:00" maxDate="2022-08-02T00:00:00"/>
     </cacheField>
     <cacheField name="Referencia" numFmtId="0">
-      <sharedItems count="5">
+      <sharedItems count="6">
         <s v="mar"/>
         <s v="abr"/>
         <s v="mai"/>
         <s v="jun"/>
         <s v="jul"/>
+        <s v="ago"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Semana" numFmtId="0">
@@ -8190,7 +8800,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="261">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="262">
   <r>
     <x v="0"/>
     <d v="2022-03-09T00:00:00"/>
@@ -11062,15 +11672,26 @@
     <d v="1899-12-30T02:59:00"/>
     <s v="Banco de Dados MySQL/MariaDB"/>
   </r>
+  <r>
+    <x v="112"/>
+    <d v="2022-08-01T00:00:00"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="16"/>
+    <d v="1899-12-30T22:04:00"/>
+    <d v="1899-12-30T22:56:00"/>
+    <d v="1899-12-30T00:52:00"/>
+    <s v="Módulo 1: (NOVO) Primeiros Passos"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tb_ranking" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="tb_ranking" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="14" showAll="0">
-      <items count="114">
+      <items count="115">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -11183,18 +11804,20 @@
         <item x="109"/>
         <item x="110"/>
         <item x="111"/>
-        <item m="1" x="112"/>
+        <item m="1" x="113"/>
+        <item x="112"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField numFmtId="165" showAll="0"/>
     <pivotField showAll="0">
-      <items count="6">
+      <items count="7">
         <item h="1" x="0"/>
         <item h="1" x="1"/>
         <item h="1" x="2"/>
         <item h="1" x="3"/>
         <item x="4"/>
+        <item h="1" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -11274,29 +11897,29 @@
     <dataField name="Soma de Total horas de estudo" fld="7" baseField="0" baseItem="0" numFmtId="166"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="66">
+    <format dxfId="90">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="65">
+    <format dxfId="89">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="64">
+    <format dxfId="88">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="63">
+    <format dxfId="87">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="62">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -11316,16 +11939,19 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tb_totalDia" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="tb_totalDia" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="114">
+      <items count="115">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -11438,18 +12064,20 @@
         <item x="109"/>
         <item x="110"/>
         <item x="111"/>
-        <item m="1" x="112"/>
+        <item m="1" x="113"/>
+        <item x="112"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField numFmtId="165" showAll="0"/>
     <pivotField showAll="0">
-      <items count="6">
+      <items count="7">
         <item h="1" x="0"/>
         <item h="1" x="1"/>
         <item h="1" x="2"/>
         <item h="1" x="3"/>
         <item x="4"/>
+        <item h="1" x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -11559,22 +12187,22 @@
     <dataField name="Soma de Total horas de estudo" fld="7" baseField="0" baseItem="0" numFmtId="166"/>
   </dataFields>
   <formats count="9">
-    <format dxfId="53">
+    <format dxfId="77">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="76">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="75">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="74">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -11632,7 +12260,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="50">
@@ -11690,7 +12318,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="12">
@@ -11710,7 +12338,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -11730,23 +12358,27 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tb_totalMes" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="tb_totalMes" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField numFmtId="165" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+      <items count="7">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
+        <item x="5"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -11760,7 +12392,7 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="7">
     <i>
       <x/>
     </i>
@@ -11776,6 +12408,9 @@
     <i>
       <x v="4"/>
     </i>
+    <i>
+      <x v="5"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -11787,29 +12422,29 @@
     <dataField name="Soma de Total horas de estudo" fld="7" baseField="0" baseItem="0" numFmtId="166"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="44">
+    <format dxfId="68">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="67">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="66">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="65">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="64">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -11829,12 +12464,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tb_totalCurso" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="tb_totalCurso" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A3:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="14" showAll="0"/>
@@ -11952,7 +12590,7 @@
     <dataField name="Soma de Total horas de estudo" fld="7" baseField="0" baseItem="0" numFmtId="166"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="37">
+    <format dxfId="61">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -11972,24 +12610,28 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Referencia" sourceName="Referencia">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Referencia" xr10:uid="{00000000-0013-0000-FFFF-FFFF01000000}" sourceName="Referencia">
   <pivotTables>
     <pivotTable tabId="3" name="tb_ranking"/>
     <pivotTable tabId="4" name="tb_totalDia"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
-      <items count="5">
+      <items count="6">
         <i x="0"/>
         <i x="1"/>
         <i x="2"/>
         <i x="3"/>
         <i x="4" s="1"/>
+        <i x="5"/>
       </items>
     </tabular>
   </data>
@@ -11997,7 +12639,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Semana" sourceName="Semana">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Semana" xr10:uid="{00000000-0013-0000-FFFF-FFFF02000000}" sourceName="Semana">
   <pivotTables>
     <pivotTable tabId="3" name="tb_ranking"/>
     <pivotTable tabId="4" name="tb_totalDia"/>
@@ -12022,14 +12664,14 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Data" sourceName="Data">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Data" xr10:uid="{00000000-0013-0000-FFFF-FFFF03000000}" sourceName="Data">
   <pivotTables>
     <pivotTable tabId="4" name="tb_totalDia"/>
     <pivotTable tabId="3" name="tb_ranking"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
-      <items count="113">
+      <items count="114">
         <i x="87" s="1"/>
         <i x="88" s="1"/>
         <i x="89" s="1"/>
@@ -12142,6 +12784,7 @@
         <i x="84" s="1" nd="1"/>
         <i x="85" s="1" nd="1"/>
         <i x="86" s="1" nd="1"/>
+        <i x="113" s="1" nd="1"/>
         <i x="112" s="1" nd="1"/>
       </items>
     </tabular>
@@ -12150,7 +12793,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Semana1" sourceName="Semana">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Semana1" xr10:uid="{00000000-0013-0000-FFFF-FFFF04000000}" sourceName="Semana">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="1" column="4"/>
@@ -12160,7 +12803,7 @@
 </file>
 
 <file path=xl/slicerCaches/slicerCache5.xml><?xml version="1.0" encoding="utf-8"?>
-<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Referencia1" sourceName="Referencia">
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Referencia1" xr10:uid="{00000000-0013-0000-FFFF-FFFF05000000}" sourceName="Referencia">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="1" column="3"/>
@@ -12170,33 +12813,33 @@
 </file>
 
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="Semana 1" cache="SegmentaçãodeDados_Semana1" caption="Semana" rowHeight="241300"/>
-  <slicer name="Referencia 1" cache="SegmentaçãodeDados_Referencia1" caption="Referencia" rowHeight="241300"/>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Semana 1" xr10:uid="{00000000-0014-0000-FFFF-FFFF01000000}" cache="SegmentaçãodeDados_Semana1" caption="Semana" rowHeight="241300"/>
+  <slicer name="Referencia 1" xr10:uid="{00000000-0014-0000-FFFF-FFFF02000000}" cache="SegmentaçãodeDados_Referencia1" caption="Referencia" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
-<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <slicer name="Referencia" cache="SegmentaçãodeDados_Referencia" caption="Referencia" columnCount="5" rowHeight="241300"/>
-  <slicer name="Semana" cache="SegmentaçãodeDados_Semana" caption="Semana" columnCount="4" rowHeight="241300"/>
-  <slicer name="Data" cache="SegmentaçãodeDados_Data" caption="Data" columnCount="19" rowHeight="288000"/>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Referencia" xr10:uid="{00000000-0014-0000-FFFF-FFFF03000000}" cache="SegmentaçãodeDados_Referencia" caption="Referencia" columnCount="6" rowHeight="241300"/>
+  <slicer name="Semana" xr10:uid="{00000000-0014-0000-FFFF-FFFF04000000}" cache="SegmentaçãodeDados_Semana" caption="Semana" columnCount="4" rowHeight="241300"/>
+  <slicer name="Data" xr10:uid="{00000000-0014-0000-FFFF-FFFF05000000}" cache="SegmentaçãodeDados_Data" caption="Data" columnCount="19" rowHeight="288000"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela1" displayName="Tabela1" ref="C1:D307" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="C1:D307" totalsRowShown="0" headerRowDxfId="83" headerRowBorderDxfId="82" tableBorderDxfId="81" totalsRowBorderDxfId="80">
   <tableColumns count="2">
-    <tableColumn id="1" name="Dia" dataDxfId="55"/>
-    <tableColumn id="2" name="Semana" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Dia" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Semana" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="baseDeDados" displayName="baseDeDados" ref="A1:I262" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="A1:I262">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="baseDeDados" displayName="baseDeDados" ref="A1:I263" totalsRowShown="0" headerRowDxfId="60" headerRowBorderDxfId="59" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+  <autoFilter ref="A1:I263" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="jul"/>
@@ -12209,17 +12852,17 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Data" dataDxfId="32"/>
-    <tableColumn id="2" name="Dia Semana" dataDxfId="31"/>
-    <tableColumn id="3" name="Referencia" dataDxfId="30"/>
-    <tableColumn id="4" name="Semana" dataDxfId="29"/>
-    <tableColumn id="5" name="Matéria" dataDxfId="28"/>
-    <tableColumn id="6" name="Inicio" dataDxfId="27"/>
-    <tableColumn id="7" name="Fim" dataDxfId="26"/>
-    <tableColumn id="8" name="Total horas de estudo" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Data" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Dia Semana" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Referencia" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Semana" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Matéria" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Inicio" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Fim" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Total horas de estudo" dataDxfId="49">
       <calculatedColumnFormula>G2-F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Assunto" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Assunto" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13049,7 +13692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:B8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -13116,7 +13759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D307"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A281" workbookViewId="0">
@@ -15602,7 +16245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:B29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -15838,8 +16481,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A3:B10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -15901,10 +16544,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3.6111111111111115E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="8">
-        <v>16.683333333333334</v>
+      <c r="B10" s="8">
+        <v>16.719444444444445</v>
       </c>
     </row>
   </sheetData>
@@ -15913,7 +16564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -15929,7 +16580,7 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="17">
         <f>GETPIVOTDATA("Total horas de estudo",$A$3)</f>
-        <v>16.683333333333337</v>
+        <v>16.719444444444445</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -15961,7 +16612,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="17">
-        <v>3.5562499999999999</v>
+        <v>3.5923611111111109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -16097,7 +16748,7 @@
         <v>119</v>
       </c>
       <c r="B23" s="17">
-        <v>16.683333333333337</v>
+        <v>16.719444444444445</v>
       </c>
     </row>
   </sheetData>
@@ -16106,11 +16757,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I262"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I263"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B265" sqref="B265"/>
+      <selection activeCell="G264" sqref="G264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23906,6 +24557,38 @@
       </c>
       <c r="I262" s="13" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A263" s="34">
+        <v>44774</v>
+      </c>
+      <c r="B263" s="10">
+        <f>baseDeDados[[#This Row],[Data]]</f>
+        <v>44774</v>
+      </c>
+      <c r="C263" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D263" s="11" t="str">
+        <f>VLOOKUP(baseDeDados[[#This Row],[Data]],Tabela1[],2,)</f>
+        <v>Semana 01</v>
+      </c>
+      <c r="E263" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F263" s="12">
+        <v>0.9194444444444444</v>
+      </c>
+      <c r="G263" s="12">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="H263" s="35">
+        <f>G263-F263</f>
+        <v>3.6111111111111205E-2</v>
+      </c>
+      <c r="I263" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -23926,14 +24609,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>